<commit_message>
Please check new updated file
</commit_message>
<xml_diff>
--- a/Pooja/Remark.xlsx
+++ b/Pooja/Remark.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/750f923d45d01bdb/Documents/Aventisia/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/750f923d45d01bdb/Desktop/public-docs/Pooja/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="174" documentId="11_F25DC773A252ABDACC104888491A68745BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CFB0512-1C51-45A0-90C0-BF5CCBC6B32B}"/>
@@ -3824,8 +3824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Please check updated md files
</commit_message>
<xml_diff>
--- a/Pooja/Remark.xlsx
+++ b/Pooja/Remark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/750f923d45d01bdb/Desktop/public-docs/Pooja/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="11_F25DC773A252ABDACC104888491A68745BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CFB0512-1C51-45A0-90C0-BF5CCBC6B32B}"/>
+  <xr:revisionPtr revIDLastSave="217" documentId="11_F25DC773A252ABDACC104888491A68745BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C43F49A3-1BE1-4912-AB62-62409B3D27A1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="111">
   <si>
     <t>Action Name</t>
   </si>
@@ -113,9 +113,6 @@
     <t>data-transformation &gt;text&gt;use-the-recognize-entity-in-text-actions</t>
   </si>
   <si>
-    <t>use-the-recognize-entity-in-text-actions</t>
-  </si>
-  <si>
     <t>convert-text-to-number</t>
   </si>
   <si>
@@ -345,6 +342,24 @@
   </si>
   <si>
     <t>ui-interface &gt; ui-automation&gt;expand-collapse-tree-node-in-window</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>recognisze-entities-in-text</t>
+  </si>
+  <si>
+    <t>not found</t>
+  </si>
+  <si>
+    <t>Setting button is not available</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Not Found</t>
   </si>
 </sst>
 </file>
@@ -368,12 +383,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -388,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -413,6 +434,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3822,10 +3856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3835,9 +3869,10 @@
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
     <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3854,7 +3889,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="142.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="142.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3869,7 +3904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="181.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="181.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -3884,7 +3919,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="139.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="139.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -3899,7 +3934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -3914,7 +3949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="170.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="170.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -3928,8 +3963,11 @@
       <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="52.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="52.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -3943,8 +3981,11 @@
       <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -3957,8 +3998,11 @@
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -3971,8 +4015,11 @@
       <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -3985,8 +4032,11 @@
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -3999,8 +4049,11 @@
       <c r="E11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -4013,8 +4066,11 @@
       <c r="E12" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -4027,10 +4083,13 @@
       <c r="E13" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>27</v>
@@ -4041,13 +4100,16 @@
       <c r="E14" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>14</v>
@@ -4055,13 +4117,16 @@
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>14</v>
@@ -4069,13 +4134,16 @@
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>14</v>
@@ -4083,13 +4151,16 @@
       <c r="E17" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>14</v>
@@ -4097,27 +4168,33 @@
       <c r="E18" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="C20" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>14</v>
@@ -4126,12 +4203,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>14</v>
@@ -4139,13 +4216,16 @@
       <c r="E21" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>14</v>
@@ -4153,13 +4233,16 @@
       <c r="E22" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>14</v>
@@ -4167,13 +4250,16 @@
       <c r="E23" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>14</v>
@@ -4181,27 +4267,33 @@
       <c r="E24" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="F24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="10" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>14</v>
@@ -4209,13 +4301,16 @@
       <c r="E26" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>14</v>
@@ -4223,13 +4318,16 @@
       <c r="E27" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>14</v>
@@ -4237,13 +4335,16 @@
       <c r="E28" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>14</v>
@@ -4251,13 +4352,16 @@
       <c r="E29" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>14</v>
@@ -4265,13 +4369,16 @@
       <c r="E30" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>14</v>
@@ -4279,13 +4386,16 @@
       <c r="E31" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>14</v>
@@ -4293,41 +4403,50 @@
       <c r="E32" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="F32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="10" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="D33" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="10" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="C34" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="E34" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="C35" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>14</v>
@@ -4335,13 +4454,16 @@
       <c r="E35" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>9</v>
@@ -4349,13 +4471,16 @@
       <c r="E36" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>9</v>
@@ -4363,13 +4488,16 @@
       <c r="E37" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>14</v>
@@ -4377,13 +4505,16 @@
       <c r="E38" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>14</v>
@@ -4391,13 +4522,16 @@
       <c r="E39" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>14</v>
@@ -4405,13 +4539,16 @@
       <c r="E40" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>14</v>
@@ -4420,12 +4557,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>14</v>
@@ -4434,12 +4571,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>14</v>
@@ -4448,12 +4585,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>14</v>
@@ -4462,12 +4599,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>14</v>
@@ -4476,12 +4613,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>14</v>
@@ -4490,12 +4627,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>14</v>
@@ -4504,12 +4641,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>14</v>
@@ -4520,10 +4657,10 @@
     </row>
     <row r="49" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>14</v>
@@ -4534,10 +4671,10 @@
     </row>
     <row r="50" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>14</v>
@@ -4548,10 +4685,10 @@
     </row>
     <row r="51" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>14</v>
@@ -4562,10 +4699,10 @@
     </row>
     <row r="52" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>14</v>
@@ -4576,10 +4713,10 @@
     </row>
     <row r="53" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>14</v>

</xml_diff>